<commit_message>
add bảng phân công công việc
</commit_message>
<xml_diff>
--- a/PhanCongCongViec.xlsx
+++ b/PhanCongCongViec.xlsx
@@ -142,9 +142,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -157,7 +158,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,7 +442,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -450,95 +451,97 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="5"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="6"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="1"/>
+      <c r="C3" s="7">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
+      <c r="A4" s="3"/>
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
+      <c r="A5" s="3"/>
       <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
+      <c r="A6" s="3"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
+      <c r="A7" s="3"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
+      <c r="A8" s="3"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
+      <c r="A9" s="3"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="3" t="s">
         <v>6</v>
       </c>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
+      <c r="A11" s="3"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
+      <c r="A12" s="3"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
+      <c r="A13" s="3"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
+      <c r="A14" s="3"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
+      <c r="A15" s="3"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>

</xml_diff>

<commit_message>
Hoàn thành tất cả. Thêm bảng phân công
</commit_message>
<xml_diff>
--- a/PhanCongCongViec.xlsx
+++ b/PhanCongCongViec.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Tên</t>
   </si>
@@ -46,12 +46,27 @@
   </si>
   <si>
     <t>Tiến độ</t>
+  </si>
+  <si>
+    <t>1. Hoàn thành layout login, register</t>
+  </si>
+  <si>
+    <t>2. Liên kết API axios, localStrorage</t>
+  </si>
+  <si>
+    <t>4. Hiển thị Name ra trang index</t>
+  </si>
+  <si>
+    <t>3. Hoàn thành sự kiện đăng nhập,  đăng xuất</t>
+  </si>
+  <si>
+    <t>5. Hoàn thành kiểm tra lỗi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -146,6 +161,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -158,7 +174,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -442,20 +457,21 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="38" customWidth="1"/>
+    <col min="2" max="2" width="42.28515625" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="42" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="6"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="7"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -469,79 +485,99 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="7">
+      <c r="C3" s="3">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
+      <c r="A4" s="4"/>
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
+      <c r="A5" s="4"/>
       <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
+      <c r="A6" s="4"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
+      <c r="A7" s="4"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
+      <c r="A8" s="4"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="3"/>
+      <c r="A9" s="4"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
+      <c r="B10" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="3"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
+      <c r="A11" s="4"/>
+      <c r="B11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
+      <c r="A12" s="4"/>
+      <c r="B12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="3"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
+      <c r="A13" s="4"/>
+      <c r="B13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
+      <c r="A14" s="4"/>
+      <c r="B14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="3">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="3"/>
+      <c r="A15" s="4"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>

</xml_diff>